<commit_message>
stream docker results (failed validation though)
</commit_message>
<xml_diff>
--- a/Stream/results/Stream.xlsx
+++ b/Stream/results/Stream.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="13480" windowWidth="16960" windowHeight="10180" tabRatio="500"/>
+    <workbookView xWindow="20780" yWindow="9260" windowWidth="16960" windowHeight="10180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -208,6 +208,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>46.3754</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.204</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.7567</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.5626</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -278,11 +290,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2145231384"/>
-        <c:axId val="-2136911400"/>
+        <c:axId val="2072262504"/>
+        <c:axId val="-2133576072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2145231384"/>
+        <c:axId val="2072262504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -291,7 +303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136911400"/>
+        <c:crossAx val="-2133576072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -299,7 +311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136911400"/>
+        <c:axId val="-2133576072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +322,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145231384"/>
+        <c:crossAx val="2072262504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -692,7 +704,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -720,6 +732,9 @@
       <c r="B4">
         <v>47.0214</v>
       </c>
+      <c r="C4">
+        <v>46.375399999999999</v>
+      </c>
       <c r="D4">
         <v>36.153399999999998</v>
       </c>
@@ -731,6 +746,9 @@
       <c r="B5">
         <v>46.751600000000003</v>
       </c>
+      <c r="C5">
+        <v>45.204000000000001</v>
+      </c>
       <c r="D5">
         <v>36.0015</v>
       </c>
@@ -742,6 +760,9 @@
       <c r="B6">
         <v>52.803699999999999</v>
       </c>
+      <c r="C6">
+        <v>50.756700000000002</v>
+      </c>
       <c r="D6">
         <v>41.684800000000003</v>
       </c>
@@ -752,6 +773,9 @@
       </c>
       <c r="B7">
         <v>52.759599999999999</v>
+      </c>
+      <c r="C7">
+        <v>51.562600000000003</v>
       </c>
       <c r="D7">
         <v>40.918999999999997</v>

</xml_diff>